<commit_message>
sensitivity and scout data added
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7118480B-8352-49BC-AAE1-A0B430B11295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19A66D8-6478-4EDE-B721-A3B52890CC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="variable_definitions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">variable_definitions!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">variable_definitions!$A$1:$F$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="157">
   <si>
     <t>Round</t>
   </si>
@@ -507,6 +507,9 @@
   </si>
   <si>
     <t>Capacity Retirements|Electricity|Storage Capacity|Average 2021-2035</t>
+  </si>
+  <si>
+    <t>Capacity Retirements|Electricity|Solar|PV</t>
   </si>
 </sst>
 </file>
@@ -858,20 +861,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-  <dimension ref="A1:F126"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -894,7 +898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -914,7 +918,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -934,7 +938,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -954,7 +958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -974,7 +978,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -994,7 +998,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1014,7 +1018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1074,7 +1078,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1114,7 +1118,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1134,7 +1138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1154,7 +1158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1194,7 +1198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1238,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1278,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1294,7 +1298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1314,7 +1318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1334,7 +1338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1345,56 +1349,56 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
       </c>
       <c r="F24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1405,136 +1409,136 @@
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
       </c>
       <c r="F27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1554,7 +1558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1565,7 +1569,7 @@
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
@@ -1574,7 +1578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1585,236 +1589,236 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E36" t="s">
         <v>9</v>
       </c>
       <c r="F36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>6</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>46</v>
-      </c>
-      <c r="E43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
-        <v>49</v>
-      </c>
-      <c r="E46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
-        <v>39</v>
-      </c>
-      <c r="E47" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1825,36 +1829,36 @@
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>40</v>
       </c>
       <c r="E48" t="s">
         <v>9</v>
       </c>
       <c r="F48" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1865,56 +1869,56 @@
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E50" t="s">
         <v>9</v>
       </c>
       <c r="F50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1925,36 +1929,36 @@
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="E53" t="s">
         <v>9</v>
       </c>
       <c r="F53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" t="s">
-        <v>51</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1965,36 +1969,36 @@
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="E55" t="s">
         <v>9</v>
       </c>
       <c r="F55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>94</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" t="s">
-        <v>62</v>
-      </c>
-      <c r="E56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2005,16 +2009,16 @@
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="E57" t="s">
         <v>9</v>
       </c>
       <c r="F57" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2034,7 +2038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -2054,7 +2058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2065,7 +2069,7 @@
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E60" t="s">
         <v>9</v>
@@ -2074,7 +2078,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -2085,7 +2089,7 @@
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>53</v>
+        <v>156</v>
       </c>
       <c r="E61" t="s">
         <v>9</v>
@@ -2094,7 +2098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -2114,7 +2118,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -2134,7 +2138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2154,7 +2158,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -2165,147 +2169,147 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
+        <v>155</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
         <v>60</v>
       </c>
-      <c r="E65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
         <v>61</v>
       </c>
-      <c r="E66" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
         <v>56</v>
       </c>
-      <c r="E67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>6</v>
-      </c>
-      <c r="B68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
         <v>145</v>
       </c>
-      <c r="E68" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
         <v>58</v>
       </c>
-      <c r="E69" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>6</v>
-      </c>
-      <c r="B70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
         <v>57</v>
       </c>
-      <c r="E70" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
         <v>79</v>
-      </c>
-      <c r="E71" t="s">
-        <v>77</v>
-      </c>
-      <c r="F71" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" t="s">
-        <v>84</v>
       </c>
       <c r="E72" t="s">
         <v>77</v>
@@ -2314,7 +2318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2325,7 +2329,7 @@
         <v>6</v>
       </c>
       <c r="D73" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E73" t="s">
         <v>77</v>
@@ -2334,7 +2338,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2345,7 +2349,7 @@
         <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E74" t="s">
         <v>77</v>
@@ -2354,27 +2358,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E75" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F75" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2385,7 +2389,7 @@
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E76" t="s">
         <v>89</v>
@@ -2394,7 +2398,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2405,16 +2409,16 @@
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="E77" t="s">
         <v>89</v>
       </c>
       <c r="F77" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2425,16 +2429,16 @@
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E78" t="s">
         <v>89</v>
       </c>
       <c r="F78" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2445,16 +2449,16 @@
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E79" t="s">
         <v>89</v>
       </c>
       <c r="F79" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2465,16 +2469,16 @@
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="E80" t="s">
         <v>89</v>
       </c>
       <c r="F80" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2485,16 +2489,16 @@
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E81" t="s">
         <v>89</v>
       </c>
       <c r="F81" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2505,16 +2509,16 @@
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E82" t="s">
         <v>89</v>
       </c>
       <c r="F82" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2525,16 +2529,16 @@
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="E83" t="s">
         <v>89</v>
       </c>
       <c r="F83" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2545,7 +2549,7 @@
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E84" t="s">
         <v>89</v>
@@ -2554,7 +2558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2565,16 +2569,16 @@
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="E85" t="s">
         <v>89</v>
       </c>
       <c r="F85" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2585,16 +2589,16 @@
         <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E86" t="s">
         <v>89</v>
       </c>
       <c r="F86" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2605,16 +2609,16 @@
         <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E87" t="s">
         <v>89</v>
       </c>
       <c r="F87" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2625,16 +2629,16 @@
         <v>6</v>
       </c>
       <c r="D88" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E88" t="s">
         <v>89</v>
       </c>
       <c r="F88" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2645,13 +2649,13 @@
         <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="E89" t="s">
         <v>89</v>
       </c>
       <c r="F89" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2665,7 +2669,7 @@
         <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E90" t="s">
         <v>89</v>
@@ -2685,7 +2689,7 @@
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E91" t="s">
         <v>89</v>
@@ -2705,7 +2709,7 @@
         <v>6</v>
       </c>
       <c r="D92" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E92" t="s">
         <v>89</v>
@@ -2725,7 +2729,7 @@
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E93" t="s">
         <v>89</v>
@@ -2745,7 +2749,7 @@
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E94" t="s">
         <v>89</v>
@@ -2765,7 +2769,7 @@
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E95" t="s">
         <v>89</v>
@@ -2785,7 +2789,7 @@
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E96" t="s">
         <v>89</v>
@@ -2805,7 +2809,7 @@
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E97" t="s">
         <v>89</v>
@@ -2825,7 +2829,7 @@
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E98" t="s">
         <v>89</v>
@@ -2845,7 +2849,7 @@
         <v>6</v>
       </c>
       <c r="D99" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E99" t="s">
         <v>89</v>
@@ -2865,16 +2869,16 @@
         <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="E100" t="s">
         <v>89</v>
       </c>
       <c r="F100" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -2885,16 +2889,16 @@
         <v>6</v>
       </c>
       <c r="D101" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E101" t="s">
         <v>89</v>
       </c>
       <c r="F101" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -2905,13 +2909,13 @@
         <v>6</v>
       </c>
       <c r="D102" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="E102" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="F102" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2925,7 +2929,7 @@
         <v>6</v>
       </c>
       <c r="D103" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="E103" t="s">
         <v>12</v>
@@ -2945,16 +2949,16 @@
         <v>6</v>
       </c>
       <c r="D104" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="E104" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="F104" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -2965,47 +2969,47 @@
         <v>6</v>
       </c>
       <c r="D105" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E105" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F105" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C106" t="s">
         <v>6</v>
       </c>
       <c r="D106" t="s">
+        <v>129</v>
+      </c>
+      <c r="E106" t="s">
+        <v>130</v>
+      </c>
+      <c r="F106" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" t="s">
         <v>97</v>
-      </c>
-      <c r="E106" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>6</v>
-      </c>
-      <c r="B107" t="s">
-        <v>7</v>
-      </c>
-      <c r="C107" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" t="s">
-        <v>90</v>
       </c>
       <c r="E107" t="s">
         <v>14</v>
@@ -3014,7 +3018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3025,36 +3029,36 @@
         <v>6</v>
       </c>
       <c r="D108" t="s">
+        <v>90</v>
+      </c>
+      <c r="E108" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>6</v>
+      </c>
+      <c r="B109" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" t="s">
         <v>91</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E109" t="s">
         <v>92</v>
       </c>
-      <c r="F108" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>6</v>
-      </c>
-      <c r="B109" t="s">
-        <v>7</v>
-      </c>
-      <c r="C109" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" t="s">
-        <v>86</v>
-      </c>
-      <c r="E109" t="s">
-        <v>14</v>
-      </c>
       <c r="F109" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3065,7 +3069,7 @@
         <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="E110" t="s">
         <v>14</v>
@@ -3074,7 +3078,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3085,7 +3089,7 @@
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="E111" t="s">
         <v>14</v>
@@ -3094,7 +3098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3105,7 +3109,7 @@
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="E112" t="s">
         <v>14</v>
@@ -3114,7 +3118,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3125,7 +3129,7 @@
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
@@ -3134,7 +3138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3145,7 +3149,7 @@
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E114" t="s">
         <v>14</v>
@@ -3154,7 +3158,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3165,7 +3169,7 @@
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>13</v>
+        <v>151</v>
       </c>
       <c r="E115" t="s">
         <v>14</v>
@@ -3174,7 +3178,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3185,7 +3189,7 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="E116" t="s">
         <v>14</v>
@@ -3194,7 +3198,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3205,7 +3209,7 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="E117" t="s">
         <v>14</v>
@@ -3214,7 +3218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E118" t="s">
         <v>14</v>
@@ -3234,7 +3238,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3245,7 +3249,7 @@
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="E119" t="s">
         <v>14</v>
@@ -3254,7 +3258,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3265,7 +3269,7 @@
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="E120" t="s">
         <v>14</v>
@@ -3274,7 +3278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -3285,7 +3289,7 @@
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="E121" t="s">
         <v>14</v>
@@ -3294,7 +3298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -3305,7 +3309,7 @@
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="E122" t="s">
         <v>14</v>
@@ -3314,7 +3318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -3325,7 +3329,7 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="E123" t="s">
         <v>14</v>
@@ -3334,7 +3338,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -3345,7 +3349,7 @@
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="E124" t="s">
         <v>14</v>
@@ -3354,7 +3358,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>6</v>
       </c>
@@ -3365,7 +3369,7 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="E125" t="s">
         <v>14</v>
@@ -3374,7 +3378,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -3385,7 +3389,7 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="E126" t="s">
         <v>14</v>
@@ -3394,9 +3398,46 @@
         <v>29</v>
       </c>
     </row>
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127" t="s">
+        <v>82</v>
+      </c>
+      <c r="E127" t="s">
+        <v>14</v>
+      </c>
+      <c r="F127" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F112">
+  <autoFilter ref="A1:F127" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Buses"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Commerical Aircraft"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Light-Duty Trucks"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Lubricants"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Medium- and Heavy-Duty Trucks"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Mortorcycles"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Other Aircraft"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Passenger Cars"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Pipelines"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Rail"/>
+        <filter val="Emissions|CO2|Energy|Demand|Transportation|GHGI|Ships and Boats"/>
+        <filter val="Emissions|GHG"/>
+        <filter val="Emissions|Non-CO2 GHG"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F126">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
New USREP-ReEDS scenario plus some other things
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sweisberg\Documents\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF1F933-A002-4F71-B606-43B99BDA0824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B74EA8-92BF-4CB4-874F-1432A19DD94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-6120" windowWidth="29040" windowHeight="15840" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
+    <workbookView xWindow="-28920" yWindow="-6120" windowWidth="29040" windowHeight="15840" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_definitions" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="172">
   <si>
     <t>Round</t>
   </si>
@@ -528,6 +528,33 @@
   </si>
   <si>
     <t>Emissions|NO2</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Industry|Electricity</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Buildings|Electricity</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Transportation|Electricity</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Industry|TotalwElec</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Transportation|TotalwElec</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Buildings|TotalwElec</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Industry|TotalDI</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Transportation|TotalDI</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|Energy|Demand|Buildings|TotalDI</t>
   </si>
 </sst>
 </file>
@@ -879,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3555,6 +3582,186 @@
         <v>29</v>
       </c>
     </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134" t="s">
+        <v>10</v>
+      </c>
+      <c r="C134" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134" t="s">
+        <v>163</v>
+      </c>
+      <c r="E134" t="s">
+        <v>89</v>
+      </c>
+      <c r="F134" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" t="s">
+        <v>165</v>
+      </c>
+      <c r="E135" t="s">
+        <v>89</v>
+      </c>
+      <c r="F135" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>6</v>
+      </c>
+      <c r="B136" t="s">
+        <v>10</v>
+      </c>
+      <c r="C136" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" t="s">
+        <v>164</v>
+      </c>
+      <c r="E136" t="s">
+        <v>89</v>
+      </c>
+      <c r="F136" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137" t="s">
+        <v>10</v>
+      </c>
+      <c r="C137" t="s">
+        <v>6</v>
+      </c>
+      <c r="D137" t="s">
+        <v>166</v>
+      </c>
+      <c r="E137" t="s">
+        <v>89</v>
+      </c>
+      <c r="F137" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" t="s">
+        <v>167</v>
+      </c>
+      <c r="E138" t="s">
+        <v>89</v>
+      </c>
+      <c r="F138" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>6</v>
+      </c>
+      <c r="B139" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" t="s">
+        <v>168</v>
+      </c>
+      <c r="E139" t="s">
+        <v>89</v>
+      </c>
+      <c r="F139" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>6</v>
+      </c>
+      <c r="B140" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" t="s">
+        <v>169</v>
+      </c>
+      <c r="E140" t="s">
+        <v>89</v>
+      </c>
+      <c r="F140" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>6</v>
+      </c>
+      <c r="B141" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" t="s">
+        <v>170</v>
+      </c>
+      <c r="E141" t="s">
+        <v>89</v>
+      </c>
+      <c r="F141" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" t="s">
+        <v>6</v>
+      </c>
+      <c r="D142" t="s">
+        <v>171</v>
+      </c>
+      <c r="E142" t="s">
+        <v>89</v>
+      </c>
+      <c r="F142" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
lts dac variable update
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sweisberg\Documents\LEEP\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B74EA8-92BF-4CB4-874F-1432A19DD94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0704A875-4450-4DE2-8273-CB57DB0757E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6120" windowWidth="29040" windowHeight="15840" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_definitions" sheetId="1" r:id="rId1"/>
@@ -908,21 +908,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -962,7 +962,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -982,7 +982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>6</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>6</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>6</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>6</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>6</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>6</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>6</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>6</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>6</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>6</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>6</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>6</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
industry energy plus markdown annotations
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sweisberg\Documents\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0704A875-4450-4DE2-8273-CB57DB0757E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A9915-916F-45BD-B003-874729090033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
+    <workbookView xWindow="-28920" yWindow="-6120" windowWidth="29040" windowHeight="15840" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_definitions" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="178">
   <si>
     <t>Round</t>
   </si>
@@ -555,6 +555,24 @@
   </si>
   <si>
     <t>Emissions|CO2|Energy|Demand|Buildings|TotalDI</t>
+  </si>
+  <si>
+    <t>Transformation Energy|Coal</t>
+  </si>
+  <si>
+    <t>Transformation Energy|Oil</t>
+  </si>
+  <si>
+    <t>Transformation Energy|Gas</t>
+  </si>
+  <si>
+    <t>Transformation Energy|Biomass</t>
+  </si>
+  <si>
+    <t>Final Energy|Industry|Gas Feedstocks</t>
+  </si>
+  <si>
+    <t>Final Energy|Industry|Oil Feedstocks</t>
   </si>
 </sst>
 </file>
@@ -906,23 +924,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -962,7 +980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -982,7 +1000,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1002,7 +1020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1042,7 +1060,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1062,7 +1080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1102,7 +1120,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1122,7 +1140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1142,7 +1160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1180,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1182,7 +1200,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1202,7 +1220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1240,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1242,7 +1260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1280,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1302,7 +1320,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1322,7 +1340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1342,7 +1360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1362,7 +1380,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1382,7 +1400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1402,7 +1420,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1422,7 +1440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1442,7 +1460,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1462,7 +1480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1482,7 +1500,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1520,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1522,7 +1540,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1542,7 +1560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1562,7 +1580,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1582,7 +1600,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1622,7 +1640,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1642,7 +1660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1662,7 +1680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1682,7 +1700,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1702,7 +1720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1722,7 +1740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1742,7 +1760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1762,7 +1780,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1782,7 +1800,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1802,7 +1820,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1822,7 +1840,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1842,7 +1860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1862,7 +1880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +1900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1902,7 +1920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1922,7 +1940,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1942,7 +1960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1962,7 +1980,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1982,7 +2000,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2002,7 +2020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -2022,7 +2040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2042,7 +2060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2062,7 +2080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2082,7 +2100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -2102,7 +2120,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2122,7 +2140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -2142,7 +2160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -2162,7 +2180,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -2182,7 +2200,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2202,7 +2220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -2222,7 +2240,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -2242,7 +2260,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2262,7 +2280,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2282,7 +2300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2302,7 +2320,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -2322,7 +2340,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2342,7 +2360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2362,7 +2380,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2382,7 +2400,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2402,7 +2420,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2422,7 +2440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2442,7 +2460,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2462,7 +2480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2482,7 +2500,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2502,7 +2520,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2522,7 +2540,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2542,7 +2560,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2562,7 +2580,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2582,7 +2600,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2602,7 +2620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2622,7 +2640,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2642,7 +2660,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2662,7 +2680,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2682,7 +2700,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2702,7 +2720,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2722,7 +2740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2742,7 +2760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2762,7 +2780,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2782,7 +2800,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2802,7 +2820,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2822,7 +2840,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2842,7 +2860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -2862,7 +2880,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -2882,7 +2900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -2902,7 +2920,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -2922,7 +2940,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -2942,7 +2960,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -2962,7 +2980,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -2982,7 +3000,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3002,7 +3020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3022,7 +3040,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -3042,7 +3060,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3062,7 +3080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3082,7 +3100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3102,7 +3120,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3122,7 +3140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3142,7 +3160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3162,7 +3180,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3182,7 +3200,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3202,7 +3220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3222,7 +3240,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3242,7 +3260,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3262,7 +3280,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3282,7 +3300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3302,7 +3320,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3322,7 +3340,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -3342,7 +3360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -3362,7 +3380,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -3382,7 +3400,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -3402,7 +3420,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>6</v>
       </c>
@@ -3422,7 +3440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -3442,7 +3460,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -3462,7 +3480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -3482,7 +3500,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>6</v>
       </c>
@@ -3502,7 +3520,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>6</v>
       </c>
@@ -3522,7 +3540,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>6</v>
       </c>
@@ -3542,7 +3560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>6</v>
       </c>
@@ -3562,7 +3580,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>6</v>
       </c>
@@ -3582,7 +3600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>6</v>
       </c>
@@ -3602,7 +3620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>6</v>
       </c>
@@ -3622,7 +3640,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>6</v>
       </c>
@@ -3642,7 +3660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -3662,7 +3680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>6</v>
       </c>
@@ -3682,7 +3700,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -3702,7 +3720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>6</v>
       </c>
@@ -3722,7 +3740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>6</v>
       </c>
@@ -3742,7 +3760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>6</v>
       </c>
@@ -3759,6 +3777,126 @@
         <v>89</v>
       </c>
       <c r="F142" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>6</v>
+      </c>
+      <c r="B143" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" t="s">
+        <v>6</v>
+      </c>
+      <c r="D143" t="s">
+        <v>172</v>
+      </c>
+      <c r="E143" t="s">
+        <v>14</v>
+      </c>
+      <c r="F143" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>6</v>
+      </c>
+      <c r="B144" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" t="s">
+        <v>6</v>
+      </c>
+      <c r="D144" t="s">
+        <v>173</v>
+      </c>
+      <c r="E144" t="s">
+        <v>14</v>
+      </c>
+      <c r="F144" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" t="s">
+        <v>6</v>
+      </c>
+      <c r="D145" t="s">
+        <v>174</v>
+      </c>
+      <c r="E145" t="s">
+        <v>14</v>
+      </c>
+      <c r="F145" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146" t="s">
+        <v>6</v>
+      </c>
+      <c r="D146" t="s">
+        <v>175</v>
+      </c>
+      <c r="E146" t="s">
+        <v>14</v>
+      </c>
+      <c r="F146" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>6</v>
+      </c>
+      <c r="B147" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147" t="s">
+        <v>6</v>
+      </c>
+      <c r="D147" t="s">
+        <v>176</v>
+      </c>
+      <c r="E147" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148" t="s">
+        <v>6</v>
+      </c>
+      <c r="D148" t="s">
+        <v>177</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
usrep reeds and other data updates
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sweisberg\Documents\LEEP\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A9915-916F-45BD-B003-874729090033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9568743A-37F1-42C5-A3DD-06FA6BBE3E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6120" windowWidth="29040" windowHeight="15840" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_definitions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">variable_definitions!$A$1:$F$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">variable_definitions!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="178">
   <si>
     <t>Round</t>
   </si>
@@ -425,9 +425,6 @@
     <t>Mt NOx/yr</t>
   </si>
   <si>
-    <t>LEEP</t>
-  </si>
-  <si>
     <t>Emissions|Sulfur|Energy|Supply|Electricity</t>
   </si>
   <si>
@@ -518,18 +515,12 @@
     <t>Emissions|GHG|Gross Total</t>
   </si>
   <si>
-    <t>Emissions|F-Gasses</t>
-  </si>
-  <si>
     <t>Emissions|CH4</t>
   </si>
   <si>
     <t>Emissions|N2O</t>
   </si>
   <si>
-    <t>Emissions|NO2</t>
-  </si>
-  <si>
     <t>Emissions|CO2|Energy|Demand|Industry|Electricity</t>
   </si>
   <si>
@@ -573,6 +564,15 @@
   </si>
   <si>
     <t>Final Energy|Industry|Oil Feedstocks</t>
+  </si>
+  <si>
+    <t>Emissions|AFOLU</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|AFOLU</t>
+  </si>
+  <si>
+    <t>Emissions|F-Gases</t>
   </si>
 </sst>
 </file>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F137" sqref="F137"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1591,7 +1591,7 @@
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
@@ -1871,7 +1871,7 @@
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E47" t="s">
         <v>9</v>
@@ -2111,7 +2111,7 @@
         <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E59" t="s">
         <v>9</v>
@@ -2151,7 +2151,7 @@
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E61" t="s">
         <v>9</v>
@@ -2231,7 +2231,7 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E65" t="s">
         <v>9</v>
@@ -2311,7 +2311,7 @@
         <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E69" t="s">
         <v>9</v>
@@ -2485,19 +2485,19 @@
         <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="E78" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="F78" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2511,13 +2511,13 @@
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="E79" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="F79" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2525,19 +2525,19 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="E80" t="s">
         <v>89</v>
       </c>
       <c r="F80" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2551,13 +2551,13 @@
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E81" t="s">
         <v>89</v>
       </c>
       <c r="F81" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2571,13 +2571,13 @@
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E82" t="s">
         <v>89</v>
       </c>
       <c r="F82" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2591,13 +2591,13 @@
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E83" t="s">
         <v>89</v>
       </c>
       <c r="F83" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2611,7 +2611,7 @@
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="E84" t="s">
         <v>89</v>
@@ -2631,13 +2631,13 @@
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="E85" t="s">
         <v>89</v>
       </c>
       <c r="F85" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2651,13 +2651,13 @@
         <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E86" t="s">
         <v>89</v>
       </c>
       <c r="F86" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2671,13 +2671,13 @@
         <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E87" t="s">
         <v>89</v>
       </c>
       <c r="F87" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2691,13 +2691,13 @@
         <v>6</v>
       </c>
       <c r="D88" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="E88" t="s">
         <v>89</v>
       </c>
       <c r="F88" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2711,13 +2711,13 @@
         <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="E89" t="s">
         <v>89</v>
       </c>
       <c r="F89" t="s">
-        <v>112</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2731,7 +2731,7 @@
         <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E90" t="s">
         <v>89</v>
@@ -2751,7 +2751,7 @@
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="E91" t="s">
         <v>89</v>
@@ -2771,13 +2771,13 @@
         <v>6</v>
       </c>
       <c r="D92" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E92" t="s">
         <v>89</v>
       </c>
       <c r="F92" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2791,7 +2791,7 @@
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="E93" t="s">
         <v>89</v>
@@ -2811,13 +2811,13 @@
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="E94" t="s">
         <v>89</v>
       </c>
       <c r="F94" t="s">
-        <v>29</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2831,13 +2831,13 @@
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="E95" t="s">
         <v>89</v>
       </c>
       <c r="F95" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2851,7 +2851,7 @@
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="E96" t="s">
         <v>89</v>
@@ -2871,7 +2871,7 @@
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="E97" t="s">
         <v>89</v>
@@ -2891,7 +2891,7 @@
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="E98" t="s">
         <v>89</v>
@@ -2911,13 +2911,13 @@
         <v>6</v>
       </c>
       <c r="D99" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="E99" t="s">
         <v>89</v>
       </c>
       <c r="F99" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2931,7 +2931,7 @@
         <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E100" t="s">
         <v>89</v>
@@ -2951,13 +2951,13 @@
         <v>6</v>
       </c>
       <c r="D101" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="E101" t="s">
         <v>89</v>
       </c>
       <c r="F101" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2971,13 +2971,13 @@
         <v>6</v>
       </c>
       <c r="D102" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="E102" t="s">
         <v>89</v>
       </c>
       <c r="F102" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2991,10 +2991,10 @@
         <v>6</v>
       </c>
       <c r="D103" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="E103" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="F103" t="s">
         <v>29</v>
@@ -3011,10 +3011,10 @@
         <v>6</v>
       </c>
       <c r="D104" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="E104" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="F104" t="s">
         <v>29</v>
@@ -3031,13 +3031,13 @@
         <v>6</v>
       </c>
       <c r="D105" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="E105" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="F105" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3051,13 +3051,13 @@
         <v>6</v>
       </c>
       <c r="D106" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="E106" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="F106" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3065,16 +3065,16 @@
         <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C107" t="s">
         <v>6</v>
       </c>
       <c r="D107" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="E107" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="F107" t="s">
         <v>29</v>
@@ -3085,16 +3085,16 @@
         <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="E108" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="F108" t="s">
         <v>29</v>
@@ -3105,16 +3105,16 @@
         <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C109" t="s">
         <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="E109" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F109" t="s">
         <v>29</v>
@@ -3125,16 +3125,16 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C110" t="s">
         <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E110" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="F110" t="s">
         <v>29</v>
@@ -3145,19 +3145,19 @@
         <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="E111" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="F111" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3165,16 +3165,16 @@
         <v>6</v>
       </c>
       <c r="B112" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C112" t="s">
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="E112" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="F112" t="s">
         <v>29</v>
@@ -3185,16 +3185,16 @@
         <v>6</v>
       </c>
       <c r="B113" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="E113" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="F113" t="s">
         <v>29</v>
@@ -3205,19 +3205,19 @@
         <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C114" t="s">
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="E114" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="F114" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3225,16 +3225,16 @@
         <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C115" t="s">
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="E115" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F115" t="s">
         <v>29</v>
@@ -3245,16 +3245,16 @@
         <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C116" t="s">
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="E116" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F116" t="s">
         <v>29</v>
@@ -3265,16 +3265,16 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C117" t="s">
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E117" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F117" t="s">
         <v>29</v>
@@ -3285,16 +3285,16 @@
         <v>6</v>
       </c>
       <c r="B118" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E118" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F118" t="s">
         <v>29</v>
@@ -3305,16 +3305,16 @@
         <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C119" t="s">
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="E119" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F119" t="s">
         <v>29</v>
@@ -3325,16 +3325,16 @@
         <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C120" t="s">
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="E120" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F120" t="s">
         <v>29</v>
@@ -3345,16 +3345,16 @@
         <v>6</v>
       </c>
       <c r="B121" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C121" t="s">
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="E121" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F121" t="s">
         <v>29</v>
@@ -3365,16 +3365,16 @@
         <v>6</v>
       </c>
       <c r="B122" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C122" t="s">
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="E122" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="F122" t="s">
         <v>29</v>
@@ -3385,16 +3385,16 @@
         <v>6</v>
       </c>
       <c r="B123" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C123" t="s">
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="E123" t="s">
-        <v>14</v>
+        <v>129</v>
       </c>
       <c r="F123" t="s">
         <v>29</v>
@@ -3411,7 +3411,7 @@
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E124" t="s">
         <v>14</v>
@@ -3431,7 +3431,7 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="E125" t="s">
         <v>14</v>
@@ -3451,10 +3451,10 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E126" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="F126" t="s">
         <v>29</v>
@@ -3471,7 +3471,7 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="E127" t="s">
         <v>14</v>
@@ -3485,16 +3485,16 @@
         <v>6</v>
       </c>
       <c r="B128" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C128" t="s">
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E128" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F128" t="s">
         <v>29</v>
@@ -3505,16 +3505,16 @@
         <v>6</v>
       </c>
       <c r="B129" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E129" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F129" t="s">
         <v>29</v>
@@ -3525,16 +3525,16 @@
         <v>6</v>
       </c>
       <c r="B130" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C130" t="s">
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="E130" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F130" t="s">
         <v>29</v>
@@ -3545,16 +3545,16 @@
         <v>6</v>
       </c>
       <c r="B131" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C131" t="s">
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E131" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F131" t="s">
         <v>29</v>
@@ -3565,16 +3565,16 @@
         <v>6</v>
       </c>
       <c r="B132" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="E132" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F132" t="s">
         <v>29</v>
@@ -3585,16 +3585,16 @@
         <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C133" t="s">
         <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="E133" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F133" t="s">
         <v>29</v>
@@ -3605,16 +3605,16 @@
         <v>6</v>
       </c>
       <c r="B134" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C134" t="s">
         <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="E134" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F134" t="s">
         <v>29</v>
@@ -3625,16 +3625,16 @@
         <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C135" t="s">
         <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="E135" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F135" t="s">
         <v>29</v>
@@ -3645,16 +3645,16 @@
         <v>6</v>
       </c>
       <c r="B136" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C136" t="s">
         <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E136" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F136" t="s">
         <v>29</v>
@@ -3665,16 +3665,16 @@
         <v>6</v>
       </c>
       <c r="B137" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C137" t="s">
         <v>6</v>
       </c>
       <c r="D137" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E137" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F137" t="s">
         <v>29</v>
@@ -3685,16 +3685,16 @@
         <v>6</v>
       </c>
       <c r="B138" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C138" t="s">
         <v>6</v>
       </c>
       <c r="D138" t="s">
-        <v>167</v>
+        <v>86</v>
       </c>
       <c r="E138" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F138" t="s">
         <v>29</v>
@@ -3705,16 +3705,16 @@
         <v>6</v>
       </c>
       <c r="B139" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C139" t="s">
         <v>6</v>
       </c>
       <c r="D139" t="s">
-        <v>168</v>
+        <v>100</v>
       </c>
       <c r="E139" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F139" t="s">
         <v>29</v>
@@ -3725,16 +3725,16 @@
         <v>6</v>
       </c>
       <c r="B140" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C140" t="s">
         <v>6</v>
       </c>
       <c r="D140" t="s">
-        <v>169</v>
+        <v>85</v>
       </c>
       <c r="E140" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F140" t="s">
         <v>29</v>
@@ -3745,16 +3745,16 @@
         <v>6</v>
       </c>
       <c r="B141" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C141" t="s">
         <v>6</v>
       </c>
       <c r="D141" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="E141" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F141" t="s">
         <v>29</v>
@@ -3765,16 +3765,16 @@
         <v>6</v>
       </c>
       <c r="B142" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C142" t="s">
         <v>6</v>
       </c>
       <c r="D142" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="E142" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F142" t="s">
         <v>29</v>
@@ -3791,7 +3791,7 @@
         <v>6</v>
       </c>
       <c r="D143" t="s">
-        <v>172</v>
+        <v>80</v>
       </c>
       <c r="E143" t="s">
         <v>14</v>
@@ -3811,7 +3811,7 @@
         <v>6</v>
       </c>
       <c r="D144" t="s">
-        <v>173</v>
+        <v>13</v>
       </c>
       <c r="E144" t="s">
         <v>14</v>
@@ -3831,7 +3831,7 @@
         <v>6</v>
       </c>
       <c r="D145" t="s">
-        <v>174</v>
+        <v>81</v>
       </c>
       <c r="E145" t="s">
         <v>14</v>
@@ -3851,7 +3851,7 @@
         <v>6</v>
       </c>
       <c r="D146" t="s">
-        <v>175</v>
+        <v>82</v>
       </c>
       <c r="E146" t="s">
         <v>14</v>
@@ -3871,7 +3871,7 @@
         <v>6</v>
       </c>
       <c r="D147" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E147" t="s">
         <v>14</v>
@@ -3891,7 +3891,7 @@
         <v>6</v>
       </c>
       <c r="D148" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E148" t="s">
         <v>14</v>
@@ -3900,7 +3900,52 @@
         <v>29</v>
       </c>
     </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>6</v>
+      </c>
+      <c r="B149" t="s">
+        <v>7</v>
+      </c>
+      <c r="C149" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" t="s">
+        <v>171</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
+      </c>
+      <c r="F149" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>6</v>
+      </c>
+      <c r="B150" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" t="s">
+        <v>170</v>
+      </c>
+      <c r="E150" t="s">
+        <v>14</v>
+      </c>
+      <c r="F150" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F150">
+      <sortCondition ref="D1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
accommodating jeffs new data
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9568743A-37F1-42C5-A3DD-06FA6BBE3E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10155AF8-EEB3-470F-94A3-7770BD59E010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_definitions" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="179">
   <si>
     <t>Round</t>
   </si>
@@ -573,6 +573,9 @@
   </si>
   <si>
     <t>Emissions|F-Gases</t>
+  </si>
+  <si>
+    <t>Energy Service|Transportation|Passenger|BEV and PHEV|Sales Share</t>
   </si>
 </sst>
 </file>
@@ -924,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J123" sqref="J123"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3940,6 +3943,26 @@
         <v>29</v>
       </c>
     </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>6</v>
+      </c>
+      <c r="B151" t="s">
+        <v>7</v>
+      </c>
+      <c r="C151" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" t="s">
+        <v>178</v>
+      </c>
+      <c r="E151" t="s">
+        <v>92</v>
+      </c>
+      <c r="F151" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F150">

</xml_diff>

<commit_message>
small updates for ev sales share variables
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10155AF8-EEB3-470F-94A3-7770BD59E010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90354C3A-E8D6-4B1B-A36F-36B2D11E3EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_definitions" sheetId="1" r:id="rId1"/>
@@ -930,20 +930,20 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F152" sqref="F152"/>
+      <selection activeCell="F158" sqref="F158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -963,7 +963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -983,7 +983,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>6</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>6</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>6</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>6</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>6</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>6</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>6</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>6</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>6</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>6</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>6</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>6</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>6</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>6</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>6</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>6</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>6</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>6</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>6</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>6</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
data update for nems and gcam
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23B95AC-2FA8-4DB8-A81C-2A5EBB0E4E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B902B9-0648-41AD-B8D2-9E8E948A20A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_definitions" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="185">
   <si>
     <t>Round</t>
   </si>
@@ -591,16 +591,32 @@
   </si>
   <si>
     <t>Emissions|CO2|Energy|Supply|Petroleum Refining|Indirect</t>
+  </si>
+  <si>
+    <t>Energy Service|Transportation|Passenger|Liquids|Sales Share</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -623,14 +639,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D01E2112-7BC8-45CC-AC4C-AB88C7473BC3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -942,23 +961,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-  <dimension ref="A1:F156"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+      <selection activeCell="F158" sqref="F158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -998,7 +1017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1018,7 +1037,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1038,7 +1057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1058,7 +1077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1078,7 +1097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1098,7 +1117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1118,7 +1137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1138,7 +1157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1158,7 +1177,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1178,7 +1197,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1198,7 +1217,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1218,7 +1237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1238,7 +1257,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1258,7 +1277,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1278,7 +1297,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1298,7 +1317,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1337,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1338,7 +1357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1358,7 +1377,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1378,7 +1397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1398,7 +1417,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1418,7 +1437,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1438,7 +1457,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1458,7 +1477,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1478,7 +1497,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1498,7 +1517,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1518,7 +1537,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1538,7 +1557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1558,7 +1577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1578,7 +1597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1598,7 +1617,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1618,7 +1637,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1638,7 +1657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1658,7 +1677,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1678,7 +1697,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1698,7 +1717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1718,7 +1737,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1738,7 +1757,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1758,7 +1777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1778,7 +1797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1798,7 +1817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1818,7 +1837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1838,7 +1857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1858,7 +1877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1878,7 +1897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1898,7 +1917,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +1937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1938,7 +1957,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1958,7 +1977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1978,7 +1997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1998,7 +2017,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2018,7 +2037,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2038,7 +2057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -2058,7 +2077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2078,7 +2097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2098,7 +2117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2118,7 +2137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -2138,7 +2157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2158,7 +2177,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -2178,7 +2197,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -2198,7 +2217,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -2218,7 +2237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2238,7 +2257,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -2258,7 +2277,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -2278,7 +2297,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2298,7 +2317,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2318,7 +2337,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2338,7 +2357,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -2358,7 +2377,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2378,7 +2397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2398,7 +2417,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2418,7 +2437,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2438,7 +2457,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2458,7 +2477,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2478,7 +2497,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2498,7 +2517,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2518,7 +2537,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2538,7 +2557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2558,7 +2577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2578,7 +2597,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2598,7 +2617,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2618,7 +2637,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2638,7 +2657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2658,7 +2677,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2678,7 +2697,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2698,7 +2717,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2718,7 +2737,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2738,7 +2757,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2758,7 +2777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2778,7 +2797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2798,7 +2817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2818,7 +2837,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2838,7 +2857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2858,7 +2877,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2878,7 +2897,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -2898,7 +2917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -2918,7 +2937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -2938,7 +2957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -2958,7 +2977,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -2978,7 +2997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -2998,7 +3017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -3018,7 +3037,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3038,7 +3057,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3058,7 +3077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -3078,7 +3097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3098,7 +3117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3118,7 +3137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3138,7 +3157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3158,7 +3177,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3178,7 +3197,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3198,7 +3217,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3218,7 +3237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3238,7 +3257,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3258,7 +3277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3278,7 +3297,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3298,7 +3317,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3318,7 +3337,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3338,7 +3357,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3358,7 +3377,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -3378,7 +3397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -3398,7 +3417,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -3418,7 +3437,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -3438,7 +3457,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>6</v>
       </c>
@@ -3458,7 +3477,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -3478,7 +3497,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -3498,7 +3517,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -3518,7 +3537,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>6</v>
       </c>
@@ -3538,7 +3557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>6</v>
       </c>
@@ -3558,7 +3577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>6</v>
       </c>
@@ -3578,7 +3597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>6</v>
       </c>
@@ -3598,7 +3617,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>6</v>
       </c>
@@ -3618,7 +3637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>6</v>
       </c>
@@ -3638,7 +3657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>6</v>
       </c>
@@ -3658,7 +3677,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>6</v>
       </c>
@@ -3678,7 +3697,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -3698,7 +3717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>6</v>
       </c>
@@ -3718,7 +3737,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -3738,7 +3757,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>6</v>
       </c>
@@ -3758,7 +3777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>6</v>
       </c>
@@ -3778,7 +3797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>6</v>
       </c>
@@ -3798,7 +3817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>6</v>
       </c>
@@ -3818,7 +3837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>6</v>
       </c>
@@ -3838,7 +3857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>6</v>
       </c>
@@ -3858,7 +3877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -3878,7 +3897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>6</v>
       </c>
@@ -3898,7 +3917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>6</v>
       </c>
@@ -3918,7 +3937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>6</v>
       </c>
@@ -3938,7 +3957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>6</v>
       </c>
@@ -3958,7 +3977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>6</v>
       </c>
@@ -3978,7 +3997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>6</v>
       </c>
@@ -3998,7 +4017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>6</v>
       </c>
@@ -4018,7 +4037,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>6</v>
       </c>
@@ -4038,7 +4057,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>6</v>
       </c>
@@ -4058,7 +4077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>6</v>
       </c>
@@ -4075,6 +4094,26 @@
         <v>14</v>
       </c>
       <c r="F156" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>6</v>
+      </c>
+      <c r="B157" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" t="s">
+        <v>6</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E157" t="s">
+        <v>92</v>
+      </c>
+      <c r="F157" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ghgi industrial process data update
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B902B9-0648-41AD-B8D2-9E8E948A20A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDE0C6E-0AB9-459D-8361-676BF244B435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="186">
   <si>
     <t>Round</t>
   </si>
@@ -594,6 +594,9 @@
   </si>
   <si>
     <t>Energy Service|Transportation|Passenger|Liquids|Sales Share</t>
+  </si>
+  <si>
+    <t>Emissions|CO2|GHGI Non-Energy and Industrial Process</t>
   </si>
 </sst>
 </file>
@@ -961,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F158"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F158" sqref="F158"/>
+      <selection activeCell="K140" sqref="K140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4117,6 +4120,26 @@
         <v>29</v>
       </c>
     </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>6</v>
+      </c>
+      <c r="B158" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" t="s">
+        <v>185</v>
+      </c>
+      <c r="E158" t="s">
+        <v>89</v>
+      </c>
+      <c r="F158" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F156">

</xml_diff>

<commit_message>
haiku sensitivity data added
</commit_message>
<xml_diff>
--- a/data-raw/template_additions.xlsx
+++ b/data-raw/template_additions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDE0C6E-0AB9-459D-8361-676BF244B435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F995423-B8CA-4099-A749-B54C7AEA79A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="623" xr2:uid="{296B8F89-8AB3-45E3-AAAD-465D75263C41}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="187">
   <si>
     <t>Round</t>
   </si>
@@ -597,6 +597,9 @@
   </si>
   <si>
     <t>Emissions|CO2|GHGI Non-Energy and Industrial Process</t>
+  </si>
+  <si>
+    <t>Carbon Sequestration|CCS|Other</t>
   </si>
 </sst>
 </file>
@@ -964,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K140" sqref="K140"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,7 +2514,7 @@
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>88</v>
+        <v>186</v>
       </c>
       <c r="E77" t="s">
         <v>89</v>
@@ -2525,16 +2528,16 @@
         <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
       <c r="E78" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="F78" t="s">
         <v>29</v>
@@ -2545,13 +2548,13 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="E79" t="s">
         <v>12</v>
@@ -2565,16 +2568,16 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="E80" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="F80" t="s">
         <v>29</v>
@@ -2585,19 +2588,19 @@
         <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="E81" t="s">
         <v>89</v>
       </c>
       <c r="F81" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2611,13 +2614,13 @@
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E82" t="s">
         <v>89</v>
       </c>
       <c r="F82" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2631,13 +2634,13 @@
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E83" t="s">
         <v>89</v>
       </c>
       <c r="F83" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2651,13 +2654,13 @@
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="E84" t="s">
         <v>89</v>
       </c>
       <c r="F84" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2671,13 +2674,13 @@
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="E85" t="s">
         <v>89</v>
       </c>
       <c r="F85" t="s">
-        <v>124</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2691,13 +2694,13 @@
         <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E86" t="s">
         <v>89</v>
       </c>
       <c r="F86" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2711,13 +2714,13 @@
         <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E87" t="s">
         <v>89</v>
       </c>
       <c r="F87" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2731,13 +2734,13 @@
         <v>6</v>
       </c>
       <c r="D88" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="E88" t="s">
         <v>89</v>
       </c>
       <c r="F88" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2751,7 +2754,7 @@
         <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E89" t="s">
         <v>89</v>
@@ -2771,7 +2774,7 @@
         <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="E90" t="s">
         <v>89</v>
@@ -2791,7 +2794,7 @@
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="E91" t="s">
         <v>89</v>
@@ -2811,7 +2814,7 @@
         <v>6</v>
       </c>
       <c r="D92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E92" t="s">
         <v>89</v>
@@ -2831,13 +2834,13 @@
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="E93" t="s">
         <v>89</v>
       </c>
       <c r="F93" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2851,13 +2854,13 @@
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="E94" t="s">
         <v>89</v>
       </c>
       <c r="F94" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2871,13 +2874,13 @@
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="E95" t="s">
         <v>89</v>
       </c>
       <c r="F95" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2891,13 +2894,13 @@
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E96" t="s">
         <v>89</v>
       </c>
       <c r="F96" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2911,13 +2914,13 @@
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>166</v>
+        <v>107</v>
       </c>
       <c r="E97" t="s">
         <v>89</v>
       </c>
       <c r="F97" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2931,7 +2934,7 @@
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E98" t="s">
         <v>89</v>
@@ -2951,7 +2954,7 @@
         <v>6</v>
       </c>
       <c r="D99" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E99" t="s">
         <v>89</v>
@@ -2971,13 +2974,13 @@
         <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="E100" t="s">
         <v>89</v>
       </c>
       <c r="F100" t="s">
-        <v>112</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2991,13 +2994,13 @@
         <v>6</v>
       </c>
       <c r="D101" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E101" t="s">
         <v>89</v>
       </c>
       <c r="F101" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3011,7 +3014,7 @@
         <v>6</v>
       </c>
       <c r="D102" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E102" t="s">
         <v>89</v>
@@ -3031,7 +3034,7 @@
         <v>6</v>
       </c>
       <c r="D103" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E103" t="s">
         <v>89</v>
@@ -3051,7 +3054,7 @@
         <v>6</v>
       </c>
       <c r="D104" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E104" t="s">
         <v>89</v>
@@ -3071,7 +3074,7 @@
         <v>6</v>
       </c>
       <c r="D105" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E105" t="s">
         <v>89</v>
@@ -3091,7 +3094,7 @@
         <v>6</v>
       </c>
       <c r="D106" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E106" t="s">
         <v>89</v>
@@ -3111,7 +3114,7 @@
         <v>6</v>
       </c>
       <c r="D107" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E107" t="s">
         <v>89</v>
@@ -3131,7 +3134,7 @@
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E108" t="s">
         <v>89</v>
@@ -3151,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E109" t="s">
         <v>89</v>
@@ -3171,7 +3174,7 @@
         <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E110" t="s">
         <v>89</v>
@@ -3191,7 +3194,7 @@
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E111" t="s">
         <v>89</v>
@@ -3211,13 +3214,13 @@
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="E112" t="s">
         <v>89</v>
       </c>
       <c r="F112" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3231,13 +3234,13 @@
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="E113" t="s">
         <v>89</v>
       </c>
       <c r="F113" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3251,7 +3254,7 @@
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E114" t="s">
         <v>89</v>
@@ -3271,7 +3274,7 @@
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="E115" t="s">
         <v>89</v>
@@ -3291,13 +3294,13 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>103</v>
+        <v>181</v>
       </c>
       <c r="E116" t="s">
         <v>89</v>
       </c>
       <c r="F116" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3311,13 +3314,13 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="E117" t="s">
         <v>89</v>
       </c>
       <c r="F117" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3331,7 +3334,7 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E118" t="s">
         <v>89</v>
@@ -3351,7 +3354,7 @@
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E119" t="s">
         <v>89</v>
@@ -3371,10 +3374,10 @@
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="E120" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="F120" t="s">
         <v>29</v>
@@ -3385,16 +3388,16 @@
         <v>6</v>
       </c>
       <c r="B121" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C121" t="s">
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="E121" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="F121" t="s">
         <v>29</v>
@@ -3411,7 +3414,7 @@
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="E122" t="s">
         <v>12</v>
@@ -3431,7 +3434,7 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="E123" t="s">
         <v>12</v>
@@ -3451,7 +3454,7 @@
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E124" t="s">
         <v>12</v>
@@ -3471,7 +3474,7 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E125" t="s">
         <v>12</v>
@@ -3491,7 +3494,7 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="E126" t="s">
         <v>12</v>
@@ -3511,10 +3514,10 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="E127" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="F127" t="s">
         <v>29</v>
@@ -3531,10 +3534,10 @@
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="E128" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="F128" t="s">
         <v>29</v>
@@ -3545,16 +3548,16 @@
         <v>6</v>
       </c>
       <c r="B129" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>178</v>
+        <v>126</v>
       </c>
       <c r="E129" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="F129" t="s">
         <v>29</v>
@@ -3565,16 +3568,16 @@
         <v>6</v>
       </c>
       <c r="B130" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C130" t="s">
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="E130" t="s">
-        <v>14</v>
+        <v>129</v>
       </c>
       <c r="F130" t="s">
         <v>29</v>
@@ -3591,10 +3594,10 @@
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>90</v>
+        <v>178</v>
       </c>
       <c r="E131" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="F131" t="s">
         <v>29</v>
@@ -3610,8 +3613,8 @@
       <c r="C132" t="s">
         <v>6</v>
       </c>
-      <c r="D132" t="s">
-        <v>91</v>
+      <c r="D132" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="E132" t="s">
         <v>92</v>
@@ -3631,7 +3634,7 @@
         <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="E133" t="s">
         <v>14</v>
@@ -3651,7 +3654,7 @@
         <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>146</v>
+        <v>90</v>
       </c>
       <c r="E134" t="s">
         <v>14</v>
@@ -3671,10 +3674,10 @@
         <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="E135" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="F135" t="s">
         <v>29</v>
@@ -3691,7 +3694,7 @@
         <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E136" t="s">
         <v>14</v>
@@ -3711,7 +3714,7 @@
         <v>6</v>
       </c>
       <c r="D137" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E137" t="s">
         <v>14</v>
@@ -3731,7 +3734,7 @@
         <v>6</v>
       </c>
       <c r="D138" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="E138" t="s">
         <v>14</v>
@@ -3751,7 +3754,7 @@
         <v>6</v>
       </c>
       <c r="D139" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E139" t="s">
         <v>14</v>
@@ -3771,7 +3774,7 @@
         <v>6</v>
       </c>
       <c r="D140" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E140" t="s">
         <v>14</v>
@@ -3791,7 +3794,7 @@
         <v>6</v>
       </c>
       <c r="D141" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E141" t="s">
         <v>14</v>
@@ -3811,7 +3814,7 @@
         <v>6</v>
       </c>
       <c r="D142" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E142" t="s">
         <v>14</v>
@@ -3831,7 +3834,7 @@
         <v>6</v>
       </c>
       <c r="D143" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E143" t="s">
         <v>14</v>
@@ -3851,7 +3854,7 @@
         <v>6</v>
       </c>
       <c r="D144" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="E144" t="s">
         <v>14</v>
@@ -3871,7 +3874,7 @@
         <v>6</v>
       </c>
       <c r="D145" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="E145" t="s">
         <v>14</v>
@@ -3891,7 +3894,7 @@
         <v>6</v>
       </c>
       <c r="D146" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="E146" t="s">
         <v>14</v>
@@ -3911,7 +3914,7 @@
         <v>6</v>
       </c>
       <c r="D147" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E147" t="s">
         <v>14</v>
@@ -3931,7 +3934,7 @@
         <v>6</v>
       </c>
       <c r="D148" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E148" t="s">
         <v>14</v>
@@ -3951,7 +3954,7 @@
         <v>6</v>
       </c>
       <c r="D149" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E149" t="s">
         <v>14</v>
@@ -3971,7 +3974,7 @@
         <v>6</v>
       </c>
       <c r="D150" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="E150" t="s">
         <v>14</v>
@@ -3991,7 +3994,7 @@
         <v>6</v>
       </c>
       <c r="D151" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E151" t="s">
         <v>14</v>
@@ -4011,7 +4014,7 @@
         <v>6</v>
       </c>
       <c r="D152" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E152" t="s">
         <v>14</v>
@@ -4031,7 +4034,7 @@
         <v>6</v>
       </c>
       <c r="D153" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="E153" t="s">
         <v>14</v>
@@ -4051,7 +4054,7 @@
         <v>6</v>
       </c>
       <c r="D154" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="E154" t="s">
         <v>14</v>
@@ -4071,7 +4074,7 @@
         <v>6</v>
       </c>
       <c r="D155" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
       <c r="E155" t="s">
         <v>14</v>
@@ -4091,7 +4094,7 @@
         <v>6</v>
       </c>
       <c r="D156" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E156" t="s">
         <v>14</v>
@@ -4110,11 +4113,11 @@
       <c r="C157" t="s">
         <v>6</v>
       </c>
-      <c r="D157" s="1" t="s">
-        <v>184</v>
+      <c r="D157" t="s">
+        <v>169</v>
       </c>
       <c r="E157" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="F157" t="s">
         <v>29</v>
@@ -4131,18 +4134,38 @@
         <v>6</v>
       </c>
       <c r="D158" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="E158" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F158" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" t="s">
+        <v>170</v>
+      </c>
+      <c r="E159" t="s">
+        <v>14</v>
+      </c>
+      <c r="F159" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{C798AC80-D9FD-49DA-ABC4-7F22007F6343}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F156">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F158">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>

</xml_diff>